<commit_message>
included inset plots: fraction of hairs and number of hairs
preliminary reponse to the comments of all reviewers added in word file
</commit_message>
<xml_diff>
--- a/Data/final/experiment_data-ladybug_adhesion.xlsx
+++ b/Data/final/experiment_data-ladybug_adhesion.xlsx
@@ -5,24 +5,28 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Documents\paper-underwater_adhesion\Data\supporting_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Documents\paper-underwater_adhesion\Data\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="summarize" sheetId="2" r:id="rId1"/>
+    <sheet name="data" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">data!$A$1:$I$171</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">data!$A$1:$I$171</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="51">
   <si>
     <t>Medium</t>
   </si>
@@ -213,6 +217,15 @@
   <si>
     <t>Insect weight (g)</t>
   </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Average of Pulloff Force (µN)</t>
+  </si>
+  <si>
+    <t>StdDev of Pulloff Force (µN)2</t>
+  </si>
 </sst>
 </file>
 
@@ -277,11 +290,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -297,6 +315,3277 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Pranav Sudersan" refreshedDate="44401.729947222222" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="170">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:P171" sheet="data"/>
+  </cacheSource>
+  <cacheFields count="16">
+    <cacheField name="Date of Experiment" numFmtId="0">
+      <sharedItems count="24">
+        <s v="08 Jul 2020"/>
+        <s v="09 Jul 2020"/>
+        <s v="11 Jul 2020"/>
+        <s v="13 Jul 2020"/>
+        <s v="16 Jul 2020"/>
+        <s v="17 Jul 2020"/>
+        <s v="22 Jul 2020"/>
+        <s v="26 Aug 2020"/>
+        <s v="27 Aug 2020"/>
+        <s v="28 Aug 2020"/>
+        <s v="30 Aug 2020"/>
+        <s v="01 Sep 2020"/>
+        <s v="05 Sep 2020"/>
+        <s v="06 Sep 2020"/>
+        <s v="09 Sep 2020"/>
+        <s v="14 Sep 2020"/>
+        <s v="14 Oct 2020"/>
+        <s v="15 Oct 2020"/>
+        <s v="19 Oct 2020"/>
+        <s v="20 Oct 2020"/>
+        <s v="22 Oct 2020"/>
+        <s v="27 Oct 2020"/>
+        <s v="30 Oct 2020"/>
+        <s v="11 Nov 2020"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Insect weight (g)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.5000000000000001E-2" maxValue="4.1099999999999998E-2"/>
+    </cacheField>
+    <cacheField name="Temperature (°C)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="24.6" maxValue="26.4"/>
+    </cacheField>
+    <cacheField name="Humidity (%)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="30.3" maxValue="45"/>
+    </cacheField>
+    <cacheField name="Medium" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Substrate" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Glass"/>
+        <s v="PFOTS"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Contact Type" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Bad contact"/>
+        <s v="Underwater: bubble"/>
+        <s v="Underwater: no bubble"/>
+        <s v="In air"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Pulloff Force (µN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="8.2455829455739149E-2" maxValue="636.25036361509569"/>
+    </cacheField>
+    <cacheField name="Friction Force (µN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="62.720056859920078" maxValue="1998.1798071403971"/>
+    </cacheField>
+    <cacheField name="Vertical Force Stdev (µN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.59336239976559968" maxValue="5.1220371862303811"/>
+    </cacheField>
+    <cacheField name="Lateral Force Stdev (µN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="1.4429270826441769" maxValue="24.93028829934978"/>
+    </cacheField>
+    <cacheField name="Adhesion Preload (µN)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="121.0451906272433" maxValue="1696.024232077365"/>
+    </cacheField>
+    <cacheField name="Contact Time (s)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Adhesion Energy (pJ)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-39.216460470415143" maxValue="42837.532701458476"/>
+    </cacheField>
+    <cacheField name="Max contact area" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0" maxValue="32880.638834565973"/>
+    </cacheField>
+    <cacheField name="Pulloff contact area (µm2)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="-211.74488140221729" maxValue="12139.05658890278"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="170">
+  <r>
+    <x v="0"/>
+    <n v="3.5400000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4.282338995205123"/>
+    <n v="98.180239545408767"/>
+    <n v="2.5655358306039968"/>
+    <n v="4.2758965373539084"/>
+    <n v="1216.133226786955"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3.5400000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.5076216049344584"/>
+    <n v="100.6718011433704"/>
+    <n v="2.177033067796911"/>
+    <n v="9.9766504436378121"/>
+    <n v="1485.889527857521"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3.5400000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1.0315162657904009"/>
+    <n v="86.814684784675592"/>
+    <n v="2.211263621309806"/>
+    <n v="11.308385013703189"/>
+    <n v="1417.743723228848"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3.5400000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.8298694446226591"/>
+    <n v="108.7024457299522"/>
+    <n v="3.053581386584113"/>
+    <n v="5.3993515994498136"/>
+    <n v="1696.024232077365"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3.5400000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3.3740592660518591"/>
+    <n v="83.685990182912064"/>
+    <n v="2.5337857448637782"/>
+    <n v="4.2206794450413536"/>
+    <n v="1124.8677002507291"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2.81E-2"/>
+    <n v="26.1"/>
+    <n v="43.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="384.10348110751693"/>
+    <n v="767.07950879532746"/>
+    <n v="3.7139007376172568"/>
+    <n v="16.421393611705771"/>
+    <n v="883.73578659425129"/>
+    <n v="1"/>
+    <n v="12230.82478378324"/>
+    <n v="21944.445000008422"/>
+    <n v="6393.04424356663"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2.81E-2"/>
+    <n v="26.1"/>
+    <n v="43.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="350.38012967638332"/>
+    <n v="722.93021120705032"/>
+    <n v="4.354173275396712"/>
+    <n v="21.12187581443164"/>
+    <n v="1135.6593076604811"/>
+    <n v="1"/>
+    <n v="11416.058705495539"/>
+    <n v="23471.708915772011"/>
+    <n v="1788.384811756614"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2.81E-2"/>
+    <n v="26.1"/>
+    <n v="43.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="345.45523161771149"/>
+    <n v="684.40213338388548"/>
+    <n v="2.999731636041584"/>
+    <n v="10.34213965287435"/>
+    <n v="1330.828138456181"/>
+    <n v="1"/>
+    <n v="10377.68877440727"/>
+    <n v="23243.234451963879"/>
+    <n v="1044.7634481556629"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2.81E-2"/>
+    <n v="26.1"/>
+    <n v="43.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="341.06882446869213"/>
+    <n v="659.24698842352529"/>
+    <n v="2.4635434189255032"/>
+    <n v="21.949254991555229"/>
+    <n v="1420.4025633874451"/>
+    <n v="1"/>
+    <n v="10425.254743389611"/>
+    <n v="23326.539756460072"/>
+    <n v="1048.703353577115"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2.81E-2"/>
+    <n v="26.1"/>
+    <n v="43.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="316.84452180614818"/>
+    <n v="568.67908437243977"/>
+    <n v="1.6320831523628201"/>
+    <n v="15.39503398515788"/>
+    <n v="1045.4359485334551"/>
+    <n v="1"/>
+    <n v="8778.3560044678761"/>
+    <n v="18943.696542269921"/>
+    <n v="305.84884793757652"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2.6700000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="338.84045152190168"/>
+    <n v="467.47992589055548"/>
+    <n v="1.7216004899371899"/>
+    <n v="10.81314987921909"/>
+    <n v="306.55787761863388"/>
+    <n v="1"/>
+    <n v="9597.6298377161784"/>
+    <n v="3943.1177461532639"/>
+    <n v="1950.230967420895"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2.6700000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="485.20341443108327"/>
+    <n v="730.31569888998229"/>
+    <n v="1.5701826160496639"/>
+    <n v="6.8566953607564152"/>
+    <n v="362.4845927731572"/>
+    <n v="1"/>
+    <n v="18517.29255344165"/>
+    <n v="7061.9699267218066"/>
+    <n v="1906.4786741352971"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2.6700000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="444.63541849468072"/>
+    <n v="675.24720292278823"/>
+    <n v="2.5646334381987308"/>
+    <n v="7.2055233267017824"/>
+    <n v="279.50000150445209"/>
+    <n v="1"/>
+    <n v="16064.332528993051"/>
+    <n v="4289.3444336163566"/>
+    <n v="1839.0825607101151"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2.6700000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="449.22120960924121"/>
+    <n v="723.5064756132648"/>
+    <n v="1.9641476914096261"/>
+    <n v="9.3251365131333035"/>
+    <n v="322.11940446462319"/>
+    <n v="1"/>
+    <n v="16076.849835903849"/>
+    <n v="4709.38594784823"/>
+    <n v="1778.3524673441641"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2.6700000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="463.39359958304749"/>
+    <n v="711.25872653285023"/>
+    <n v="2.817558042032831"/>
+    <n v="4.83658286710138"/>
+    <n v="337.51434759780801"/>
+    <n v="1"/>
+    <n v="15723.154190576461"/>
+    <n v="4658.4185674602613"/>
+    <n v="1543.699718597733"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="356.73784248696779"/>
+    <n v="537.60841343064749"/>
+    <n v="2.690551748072374"/>
+    <n v="7.5526398234047916"/>
+    <n v="504.68402538358032"/>
+    <n v="1"/>
+    <n v="12282.75526180278"/>
+    <n v="21984.16440679353"/>
+    <n v="8499.3685975724129"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="367.77725168305841"/>
+    <n v="536.63920254670757"/>
+    <n v="3.5684532949101402"/>
+    <n v="12.57060847175822"/>
+    <n v="620.56319190037516"/>
+    <n v="1"/>
+    <n v="13122.438752074549"/>
+    <n v="23126.53672583419"/>
+    <n v="8414.4881292007158"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="370.57453667297648"/>
+    <n v="424.24799463448198"/>
+    <n v="5.1220371862303811"/>
+    <n v="8.0225194116086627"/>
+    <n v="439.45825264331148"/>
+    <n v="1"/>
+    <n v="11527.07378106288"/>
+    <n v="18663.551699723648"/>
+    <n v="8013.7751460870468"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="358.38998144587651"/>
+    <n v="478.87110760628372"/>
+    <n v="2.8659128607290021"/>
+    <n v="5.1712304124106838"/>
+    <n v="538.66874250775334"/>
+    <n v="1"/>
+    <n v="11515.816298358881"/>
+    <n v="19760.932124352861"/>
+    <n v="7346.3016803203027"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="31.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="354.50285283919521"/>
+    <n v="566.0471849161803"/>
+    <n v="2.768553550604206"/>
+    <n v="12.10805556938729"/>
+    <n v="609.78132342713775"/>
+    <n v="1"/>
+    <n v="12849.880122987721"/>
+    <n v="21754.635445460131"/>
+    <n v="6844.3255400400094"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2.5000000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="629.47126243591879"/>
+    <n v="1787.933525150954"/>
+    <n v="2.2149223782765599"/>
+    <n v="5.4524340653259529"/>
+    <n v="402.03009436282531"/>
+    <n v="1"/>
+    <n v="42837.532701458476"/>
+    <n v="8299.2470230366125"/>
+    <n v="539.55315884279958"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2.5000000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="622.46645568182339"/>
+    <n v="1949.769592903255"/>
+    <n v="2.3451796625129031"/>
+    <n v="11.432655411624181"/>
+    <n v="499.01739356758662"/>
+    <n v="1"/>
+    <n v="41518.445815059589"/>
+    <n v="7386.755164504445"/>
+    <n v="295.38566371569198"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2.5000000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="561.83618579448637"/>
+    <n v="1865.6569670967549"/>
+    <n v="2.0700215189182809"/>
+    <n v="12.763338105044451"/>
+    <n v="685.37273823995417"/>
+    <n v="1"/>
+    <n v="36672.280916126947"/>
+    <n v="6460.9063373188774"/>
+    <n v="140.04235589537859"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2.5000000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="590.01642556437946"/>
+    <n v="1998.1798071403971"/>
+    <n v="2.0613786109658969"/>
+    <n v="13.8842567139835"/>
+    <n v="629.36448256325093"/>
+    <n v="1"/>
+    <n v="39321.665079870967"/>
+    <n v="5220.8172476033551"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2.5000000000000001E-2"/>
+    <n v="26"/>
+    <n v="43.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="492.9901873071405"/>
+    <n v="1053.6249367122509"/>
+    <n v="2.1510670598858961"/>
+    <n v="22.9366424998552"/>
+    <n v="906.19975516358716"/>
+    <n v="1"/>
+    <n v="28365.317644105191"/>
+    <n v="4016.932572922045"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3.3599999999999998E-2"/>
+    <n v="26"/>
+    <n v="41.2"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="370.79605160036579"/>
+    <n v="601.02743904367162"/>
+    <n v="2.0359378945335158"/>
+    <n v="4.8498524324512431"/>
+    <n v="485.75127238038078"/>
+    <n v="1"/>
+    <n v="15430.102871773841"/>
+    <n v="5769.5074599179616"/>
+    <n v="1959.525361755283"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3.3599999999999998E-2"/>
+    <n v="26"/>
+    <n v="41.2"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="529.25524853563661"/>
+    <n v="886.76382702821638"/>
+    <n v="1.82627688307804"/>
+    <n v="8.9279323950524621"/>
+    <n v="488.59642057756338"/>
+    <n v="1"/>
+    <n v="24034.25187563289"/>
+    <n v="7010.6510471587508"/>
+    <n v="2936.8717580983171"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3.3599999999999998E-2"/>
+    <n v="26"/>
+    <n v="41.2"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="594.36640362382263"/>
+    <n v="971.29103721488036"/>
+    <n v="1.741204899171835"/>
+    <n v="6.2713721253618493"/>
+    <n v="392.69777190913629"/>
+    <n v="1"/>
+    <n v="28228.26421778728"/>
+    <n v="7656.3550317980398"/>
+    <n v="3088.3501140474532"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3.3599999999999998E-2"/>
+    <n v="26"/>
+    <n v="41.2"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="605.10834637400546"/>
+    <n v="1089.7020631576411"/>
+    <n v="2.0178335756729768"/>
+    <n v="5.0762913939044072"/>
+    <n v="614.83308373505076"/>
+    <n v="1"/>
+    <n v="31212.861056555332"/>
+    <n v="8350.9174017747609"/>
+    <n v="2653.6698335564129"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="3.3599999999999998E-2"/>
+    <n v="26"/>
+    <n v="41.2"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="632.73984494544311"/>
+    <n v="1133.2557287526879"/>
+    <n v="2.4250213515818171"/>
+    <n v="7.0714627980545792"/>
+    <n v="505.18784994000572"/>
+    <n v="1"/>
+    <n v="32186.47997587936"/>
+    <n v="8357.5958861014606"/>
+    <n v="2956.1783977614959"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="30.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="354.21659776865232"/>
+    <n v="318.85695733048709"/>
+    <n v="2.3344510080894421"/>
+    <n v="3.4055564650147359"/>
+    <n v="208.7627878944844"/>
+    <n v="1"/>
+    <n v="15567.661857147141"/>
+    <n v="17483.568968948421"/>
+    <n v="10994.987038740441"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="30.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="452.3233932640365"/>
+    <n v="319.828262413223"/>
+    <n v="2.0594134497453491"/>
+    <n v="3.4685175121593992"/>
+    <n v="221.5014842628332"/>
+    <n v="1"/>
+    <n v="20520.688558175971"/>
+    <n v="17415.729628156161"/>
+    <n v="10307.09047514194"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="30.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="636.25036361509569"/>
+    <n v="554.57637873420936"/>
+    <n v="1.227488172469078"/>
+    <n v="5.2209475496053441"/>
+    <n v="280.26602851293512"/>
+    <n v="1"/>
+    <n v="39665.694407300129"/>
+    <n v="18960.92000184931"/>
+    <n v="6762.4974372141296"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="30.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="547.64787510290898"/>
+    <n v="431.37839526479729"/>
+    <n v="1.5316967089501179"/>
+    <n v="11.30911004888986"/>
+    <n v="242.52944267595279"/>
+    <n v="1"/>
+    <n v="30415.153209351531"/>
+    <n v="16960.889695590431"/>
+    <n v="6517.4818540129654"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.9"/>
+    <n v="30.3"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="614.58764144813381"/>
+    <n v="542.59768476300269"/>
+    <n v="1.8717839670803409"/>
+    <n v="13.636909385410069"/>
+    <n v="330.25975779442291"/>
+    <n v="1"/>
+    <n v="37185.66445503915"/>
+    <n v="20106.455813465771"/>
+    <n v="6784.2903261979263"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="335.79123397458949"/>
+    <n v="700.09267527073439"/>
+    <n v="1.9835726811894341"/>
+    <n v="7.7892246956357374"/>
+    <n v="334.75585891730668"/>
+    <n v="1"/>
+    <n v="31062.473286895562"/>
+    <n v="24669.969603651891"/>
+    <n v="4884.2656014283284"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="386.15054015873892"/>
+    <n v="1000.658443461927"/>
+    <n v="1.228528072382941"/>
+    <n v="3.5341695629551362"/>
+    <n v="381.62946771133733"/>
+    <n v="1"/>
+    <n v="40176.941762643357"/>
+    <n v="26838.3680147786"/>
+    <n v="5787.5413219134498"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="280.23651028341311"/>
+    <n v="735.82673729258556"/>
+    <n v="1.963720264408344"/>
+    <n v="5.3555957862689514"/>
+    <n v="490.87415997327781"/>
+    <n v="1"/>
+    <n v="24666.468484974401"/>
+    <n v="28209.566296802481"/>
+    <n v="8376.0408569702704"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="297.78948912619262"/>
+    <n v="706.71949110659443"/>
+    <n v="1.3239056769646109"/>
+    <n v="10.43141015935184"/>
+    <n v="356.47595925401129"/>
+    <n v="1"/>
+    <n v="24862.795885946882"/>
+    <n v="25478.417706357581"/>
+    <n v="5518.2935511114874"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="234.3940886837033"/>
+    <n v="419.70596087398019"/>
+    <n v="1.640632719034163"/>
+    <n v="5.2086593963366177"/>
+    <n v="317.90289999779702"/>
+    <n v="1"/>
+    <n v="14101.259899012621"/>
+    <n v="22230.916827706311"/>
+    <n v="7741.3626675672886"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="11.10730055510356"/>
+    <n v="290.47434177797783"/>
+    <n v="2.96508531178835"/>
+    <n v="5.2838549107979258"/>
+    <n v="511.19908305423172"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="6.4268722771852236"/>
+    <n v="279.10372344362349"/>
+    <n v="1.884016386895039"/>
+    <n v="4.2598200515863507"/>
+    <n v="554.49058384508726"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3.8552720515002652"/>
+    <n v="242.35230195234359"/>
+    <n v="1.585562802314707"/>
+    <n v="13.3701436826739"/>
+    <n v="566.34043691475335"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4.0199919264431401"/>
+    <n v="213.74370526762141"/>
+    <n v="1.7556074252486289"/>
+    <n v="4.2071090399575359"/>
+    <n v="573.45371638495715"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="2.7099999999999999E-2"/>
+    <n v="26.1"/>
+    <n v="36.799999999999997"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="6.0064577100765746"/>
+    <n v="216.85032073742519"/>
+    <n v="1.9408613389780489"/>
+    <n v="6.1414966760674528"/>
+    <n v="578.76986742475071"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3.4000000000000002E-2"/>
+    <n v="26.4"/>
+    <n v="34.6"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="295.73939242035112"/>
+    <n v="420.83724898433678"/>
+    <n v="1.673076162848959"/>
+    <n v="7.8150411770917252"/>
+    <n v="267.56265490883499"/>
+    <n v="1"/>
+    <n v="8834.1631719907018"/>
+    <n v="5465.4606734656008"/>
+    <n v="1027.589544208935"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3.4000000000000002E-2"/>
+    <n v="26.4"/>
+    <n v="34.6"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="342.19663012196952"/>
+    <n v="464.90007005519828"/>
+    <n v="2.0020198024263558"/>
+    <n v="6.8904213419047444"/>
+    <n v="256.72039475478869"/>
+    <n v="1"/>
+    <n v="10979.4910093202"/>
+    <n v="5612.7388278280723"/>
+    <n v="1404.6179352420129"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3.4000000000000002E-2"/>
+    <n v="26.4"/>
+    <n v="34.6"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="404.25294629454692"/>
+    <n v="494.22579277482367"/>
+    <n v="2.0208349826059768"/>
+    <n v="10.81848767975052"/>
+    <n v="292.50262305547301"/>
+    <n v="1"/>
+    <n v="13759.266774454511"/>
+    <n v="6306.9496986297036"/>
+    <n v="2624.996222710467"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3.4000000000000002E-2"/>
+    <n v="26.4"/>
+    <n v="34.6"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="395.53265990593502"/>
+    <n v="490.69363176167508"/>
+    <n v="1.972911559775177"/>
+    <n v="11.651979642802729"/>
+    <n v="265.25445690088361"/>
+    <n v="1"/>
+    <n v="12110.889501628881"/>
+    <n v="5897.8046588256038"/>
+    <n v="2078.9274813136171"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <n v="3.4000000000000002E-2"/>
+    <n v="26.4"/>
+    <n v="34.6"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="635.33014861155152"/>
+    <n v="959.35768477736156"/>
+    <n v="2.56926345513503"/>
+    <n v="6.9597515588299084"/>
+    <n v="330.7322839434662"/>
+    <n v="1"/>
+    <n v="29915.540474091002"/>
+    <n v="9832.8379239518108"/>
+    <n v="3508.4201927437489"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="338.20891562992762"/>
+    <n v="1384.253269891906"/>
+    <n v="1.5463098531027879"/>
+    <n v="4.2639229268622501"/>
+    <n v="770.72847972928923"/>
+    <n v="1"/>
+    <n v="8391.2535589184499"/>
+    <n v="32880.638834565973"/>
+    <n v="10107.01630866192"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="347.52857127566722"/>
+    <n v="1332.8930396436799"/>
+    <n v="2.5871312492007452"/>
+    <n v="6.0897198511692867"/>
+    <n v="894.62296068589433"/>
+    <n v="1"/>
+    <n v="7868.922352784728"/>
+    <n v="31916.476597295648"/>
+    <n v="10072.88790967042"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="368.49186801952249"/>
+    <n v="1009.77198568889"/>
+    <n v="1.8552734402603019"/>
+    <n v="7.9968429978527684"/>
+    <n v="700.12702044826869"/>
+    <n v="1"/>
+    <n v="7647.909770796984"/>
+    <n v="28347.353973437541"/>
+    <n v="10328.02122997697"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="370.49282380880641"/>
+    <n v="1090.3925671675941"/>
+    <n v="1.5100353816514249"/>
+    <n v="6.7200697025570904"/>
+    <n v="666.59265799114064"/>
+    <n v="1"/>
+    <n v="8822.7449859260469"/>
+    <n v="28517.47957418083"/>
+    <n v="10498.44606754792"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="378.24976090065798"/>
+    <n v="1274.1602045442171"/>
+    <n v="1.3265161226935831"/>
+    <n v="8.9792831078429529"/>
+    <n v="780.35719335626482"/>
+    <n v="1"/>
+    <n v="9112.7387574249024"/>
+    <n v="30663.030538926731"/>
+    <n v="10071.54755001354"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5.3204785504270262"/>
+    <n v="158.6187774403256"/>
+    <n v="1.766891498099131"/>
+    <n v="9.7092916171907167"/>
+    <n v="866.87469473544661"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2.1548793342791441"/>
+    <n v="84.705896556930369"/>
+    <n v="2.19030526598474"/>
+    <n v="9.8025601738110684"/>
+    <n v="883.0798289264992"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="8.4776024978895084"/>
+    <n v="89.108798460750222"/>
+    <n v="2.334697389507538"/>
+    <n v="6.3084198510309069"/>
+    <n v="874.42404819637613"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3.5558970722496501"/>
+    <n v="79.4672231194604"/>
+    <n v="2.2110234485696489"/>
+    <n v="5.6008065749082458"/>
+    <n v="874.04896382624599"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <n v="3.8899999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="36.200000000000003"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1.94470834183943"/>
+    <n v="85.560033159097657"/>
+    <n v="1.996831074466596"/>
+    <n v="3.6826269264974409"/>
+    <n v="875.3562529181113"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3.44E-2"/>
+    <n v="26.1"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="314.5747576138499"/>
+    <n v="581.86218315720771"/>
+    <n v="2.4700440583138081"/>
+    <n v="5.1807702410198004"/>
+    <n v="302.53100371006371"/>
+    <n v="1"/>
+    <n v="11153.99462858779"/>
+    <n v="2266.8181801517571"/>
+    <n v="860.83717521130689"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3.44E-2"/>
+    <n v="26.1"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="301.33666537127709"/>
+    <n v="597.56342975672123"/>
+    <n v="2.3615537597081402"/>
+    <n v="11.663660976329471"/>
+    <n v="340.72590638912931"/>
+    <n v="1"/>
+    <n v="11943.8165926818"/>
+    <n v="2656.9822645010281"/>
+    <n v="57.217953393085281"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3.44E-2"/>
+    <n v="26.1"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="339.75390569635778"/>
+    <n v="612.02431837126642"/>
+    <n v="2.203045222760093"/>
+    <n v="13.993732195550979"/>
+    <n v="292.55214356923602"/>
+    <n v="1"/>
+    <n v="12660.272734967501"/>
+    <n v="4010.6055877704362"/>
+    <n v="1088.237788113905"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3.44E-2"/>
+    <n v="26.1"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="387.87222901313669"/>
+    <n v="558.55894532181037"/>
+    <n v="2.4848827617616922"/>
+    <n v="14.01967884523977"/>
+    <n v="262.11298313949681"/>
+    <n v="1"/>
+    <n v="13501.28108480978"/>
+    <n v="4833.4651566548"/>
+    <n v="1576.591115251729"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <n v="3.44E-2"/>
+    <n v="26.1"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="387.49651581112357"/>
+    <n v="668.93887187557038"/>
+    <n v="2.6334914919578551"/>
+    <n v="7.3057652346091828"/>
+    <n v="358.41437686508073"/>
+    <n v="1"/>
+    <n v="15901.44882596312"/>
+    <n v="3937.142260176744"/>
+    <n v="62.426895036934177"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="513.51366176438432"/>
+    <n v="656.93655317247078"/>
+    <n v="1.9813931313491411"/>
+    <n v="11.655108633117701"/>
+    <n v="623.09849152921618"/>
+    <n v="1"/>
+    <n v="16583.96127757807"/>
+    <n v="25860.848808854891"/>
+    <n v="12139.05658890278"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="524.5055738890087"/>
+    <n v="622.57536094935995"/>
+    <n v="1.866499407036099"/>
+    <n v="6.5124079629685321"/>
+    <n v="477.58521775584921"/>
+    <n v="1"/>
+    <n v="16415.875143092078"/>
+    <n v="23217.92651135744"/>
+    <n v="6576.4492016100576"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="561.94728820659475"/>
+    <n v="511.32360546614058"/>
+    <n v="2.1482351692501029"/>
+    <n v="5.6658836501795147"/>
+    <n v="306.56086940378668"/>
+    <n v="1"/>
+    <n v="14313.169617552579"/>
+    <n v="17503.604421928521"/>
+    <n v="6348.1630635657602"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="597.63410394116306"/>
+    <n v="530.98226062532149"/>
+    <n v="1.380622307707005"/>
+    <n v="7.0618920798048306"/>
+    <n v="277.56940469505048"/>
+    <n v="1"/>
+    <n v="14090.330551128791"/>
+    <n v="17254.040007615022"/>
+    <n v="6606.7227157293482"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="626.99599193470829"/>
+    <n v="714.6751842211138"/>
+    <n v="1.472781849751188"/>
+    <n v="5.3523175642704466"/>
+    <n v="377.05047373487622"/>
+    <n v="1"/>
+    <n v="17239.242779812939"/>
+    <n v="21515.616006399308"/>
+    <n v="6976.2870936190848"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="315.83675531551512"/>
+    <n v="420.77892210495162"/>
+    <n v="1.619668172339632"/>
+    <n v="9.8096831440266232"/>
+    <n v="622.35646515930193"/>
+    <n v="1"/>
+    <n v="7536.8144907437309"/>
+    <n v="7573.7527256520216"/>
+    <n v="788.33409038837567"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="348.77865031037078"/>
+    <n v="496.71146086613089"/>
+    <n v="2.3291063520842079"/>
+    <n v="10.73719042056177"/>
+    <n v="496.5537849105072"/>
+    <n v="1"/>
+    <n v="7406.5102399685893"/>
+    <n v="1244.658578991684"/>
+    <n v="380.35471803767871"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="349.62420718300177"/>
+    <n v="563.55921897743792"/>
+    <n v="1.680983820551605"/>
+    <n v="12.194841007053141"/>
+    <n v="482.0450281319446"/>
+    <n v="1"/>
+    <n v="8698.6493532978311"/>
+    <n v="1210.2116598329189"/>
+    <n v="329.72583348295092"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="415.04065160421618"/>
+    <n v="606.09753162976176"/>
+    <n v="2.368309329126725"/>
+    <n v="9.5742115835021302"/>
+    <n v="650.75729642937677"/>
+    <n v="1"/>
+    <n v="11735.29912192524"/>
+    <n v="1175.7647406741551"/>
+    <n v="436.93675471620139"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <n v="3.1199999999999999E-2"/>
+    <n v="25.9"/>
+    <n v="36.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="499.68809624082229"/>
+    <n v="624.1168145788979"/>
+    <n v="1.4529522910271999"/>
+    <n v="5.9289984195913652"/>
+    <n v="611.74086983508107"/>
+    <n v="1"/>
+    <n v="13493.405390328289"/>
+    <n v="1233.059106213733"/>
+    <n v="525.28930128531408"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="503.56112130652372"/>
+    <n v="504.68819837227329"/>
+    <n v="2.3588251777965961"/>
+    <n v="3.7655318037601249"/>
+    <n v="137.45279876414779"/>
+    <n v="1"/>
+    <n v="11517.566549540859"/>
+    <n v="14198.10617938748"/>
+    <n v="6814.3983277019279"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="439.63808866167813"/>
+    <n v="439.2477564187738"/>
+    <n v="2.12109168326747"/>
+    <n v="4.8685606236470447"/>
+    <n v="141.76194211072189"/>
+    <n v="1"/>
+    <n v="11102.325139215751"/>
+    <n v="13328.49722021623"/>
+    <n v="7960.0907951420959"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="497.26098594348377"/>
+    <n v="573.67032487844199"/>
+    <n v="2.2226105318233502"/>
+    <n v="4.8562932402796584"/>
+    <n v="200.1556505498431"/>
+    <n v="1"/>
+    <n v="15161.270322072671"/>
+    <n v="16718.355264778718"/>
+    <n v="6992.8817932764377"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="526.31030115140845"/>
+    <n v="560.96061179772107"/>
+    <n v="1.4900403168102769"/>
+    <n v="4.0373005807521167"/>
+    <n v="159.27081065279771"/>
+    <n v="1"/>
+    <n v="15522.963289575469"/>
+    <n v="16879.693386144769"/>
+    <n v="6995.5661616395309"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="484.78356532091431"/>
+    <n v="493.7601675681326"/>
+    <n v="0.74145429096567794"/>
+    <n v="6.0260928105085148"/>
+    <n v="137.90860857325299"/>
+    <n v="1"/>
+    <n v="12884.890205604799"/>
+    <n v="13305.649773835419"/>
+    <n v="7153.6152157351144"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="54.850308600509663"/>
+    <n v="262.11141752057978"/>
+    <n v="2.770137670233638"/>
+    <n v="8.8737054922363825"/>
+    <n v="406.7548420169407"/>
+    <n v="1"/>
+    <n v="510.97432957046777"/>
+    <n v="3604.9755397172298"/>
+    <n v="443.17925678529048"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="48.42348080487352"/>
+    <n v="252.94563729337281"/>
+    <n v="2.5070205555494569"/>
+    <n v="11.991680762632649"/>
+    <n v="532.70809093464084"/>
+    <n v="1"/>
+    <n v="451.24958336969661"/>
+    <n v="3220.4354421693888"/>
+    <n v="143.68542735782"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="58.180873362989587"/>
+    <n v="279.98541380051171"/>
+    <n v="2.721847174073142"/>
+    <n v="6.4764277960970142"/>
+    <n v="501.28037034736542"/>
+    <n v="1"/>
+    <n v="443.88014475936973"/>
+    <n v="3441.1769241255538"/>
+    <n v="741.55670819448108"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="50.016432688473529"/>
+    <n v="268.34223297673998"/>
+    <n v="2.1814609741872482"/>
+    <n v="15.042526316610481"/>
+    <n v="466.48918667006018"/>
+    <n v="1"/>
+    <n v="404.46594689829448"/>
+    <n v="4275.6359657878684"/>
+    <n v="905.28172623162573"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <n v="3.2000000000000001E-2"/>
+    <n v="25.7"/>
+    <n v="38.6"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="60.782157483610611"/>
+    <n v="244.59979553880379"/>
+    <n v="2.39261683140449"/>
+    <n v="7.8826048797910886"/>
+    <n v="463.99961917790091"/>
+    <n v="1"/>
+    <n v="534.63534553211537"/>
+    <n v="4691.8109890937576"/>
+    <n v="659.55321843843183"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="449.78358606962041"/>
+    <n v="617.36397317429567"/>
+    <n v="1.79404585310376"/>
+    <n v="6.8502684892121426"/>
+    <n v="259.49892682807001"/>
+    <n v="1"/>
+    <n v="13547.106667237809"/>
+    <n v="19127.530610841699"/>
+    <n v="5489.3893478658756"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="420.22419855483793"/>
+    <n v="675.93395099194379"/>
+    <n v="1.8503570346845619"/>
+    <n v="6.3276857506760464"/>
+    <n v="340.3646054044392"/>
+    <n v="1"/>
+    <n v="13337.727984561559"/>
+    <n v="21677.305626940451"/>
+    <n v="6055.6498523268774"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="468.45965062830442"/>
+    <n v="732.72304440973448"/>
+    <n v="2.0217255339649949"/>
+    <n v="10.358933645510049"/>
+    <n v="330.39557773472239"/>
+    <n v="1"/>
+    <n v="15733.87650526277"/>
+    <n v="21293.1170285677"/>
+    <n v="4360.9090082544208"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="492.24043461324851"/>
+    <n v="683.77766141076927"/>
+    <n v="2.0689468297068832"/>
+    <n v="9.3643326745022364"/>
+    <n v="241.35947316930279"/>
+    <n v="1"/>
+    <n v="15782.54152727904"/>
+    <n v="18635.43176571649"/>
+    <n v="4832.7928420922399"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="472.31286105736922"/>
+    <n v="651.16333267810342"/>
+    <n v="2.0717118406270041"/>
+    <n v="3.4821018907925652"/>
+    <n v="226.09524470176169"/>
+    <n v="1"/>
+    <n v="14741.70085244461"/>
+    <n v="18402.387812632202"/>
+    <n v="4902.0778809711856"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="127.30721698942089"/>
+    <n v="220.20208177438869"/>
+    <n v="2.7052678314856542"/>
+    <n v="13.418958848259591"/>
+    <n v="815.76239697417918"/>
+    <n v="1"/>
+    <n v="1559.7723193201409"/>
+    <n v="7304.8558567086066"/>
+    <n v="2064.8102309180449"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="125.65759147968311"/>
+    <n v="199.39256042757091"/>
+    <n v="3.329104642317493"/>
+    <n v="6.494705646821866"/>
+    <n v="519.54223695080714"/>
+    <n v="1"/>
+    <n v="1401.038422648505"/>
+    <n v="5444.722222135324"/>
+    <n v="2071.6334002397748"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="109.5672575701844"/>
+    <n v="173.93047619362051"/>
+    <n v="2.3194904966059919"/>
+    <n v="9.2641266997902747"/>
+    <n v="425.07998305057981"/>
+    <n v="1"/>
+    <n v="898.76556384169771"/>
+    <n v="5210.9752707008511"/>
+    <n v="1548.6474908660171"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="30.97723952359695"/>
+    <n v="123.756835227271"/>
+    <n v="2.8619976159858518"/>
+    <n v="17.31377888084641"/>
+    <n v="187.67016519342249"/>
+    <n v="1"/>
+    <n v="86.631140707967447"/>
+    <n v="3138.1846351984618"/>
+    <n v="580.9881890955163"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <n v="3.6400000000000002E-2"/>
+    <n v="25.7"/>
+    <n v="31.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="115.2236852560882"/>
+    <n v="231.27496370117299"/>
+    <n v="1.289376798062734"/>
+    <n v="10.92708583516286"/>
+    <n v="622.36740627440463"/>
+    <n v="1"/>
+    <n v="1126.700045818973"/>
+    <n v="5446.8312171858624"/>
+    <n v="1580.0387633180219"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="379.94160242406127"/>
+    <n v="914.04230258304028"/>
+    <n v="1.5288019959767269"/>
+    <n v="5.7564763246284194"/>
+    <n v="515.48630541271052"/>
+    <n v="1"/>
+    <n v="10519.534412237001"/>
+    <n v="17997.81226210426"/>
+    <n v="8387.2939486179293"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="440.90780022564837"/>
+    <n v="1213.5749447289249"/>
+    <n v="1.581448095107056"/>
+    <n v="10.919430494955551"/>
+    <n v="560.5780697275186"/>
+    <n v="1"/>
+    <n v="13827.81075639647"/>
+    <n v="19403.457463286901"/>
+    <n v="8933.2129348195012"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="404.75870093559388"/>
+    <n v="613.01285193027525"/>
+    <n v="2.1677381240680962"/>
+    <n v="5.7862018274829499"/>
+    <n v="365.8014409724118"/>
+    <n v="1"/>
+    <n v="10168.144399897221"/>
+    <n v="14670.872569882769"/>
+    <n v="8078.0133854601754"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="308.5571016616895"/>
+    <n v="437.82247752403418"/>
+    <n v="1.5079932774036151"/>
+    <n v="5.1235672725773291"/>
+    <n v="384.6628660203578"/>
+    <n v="1"/>
+    <n v="6411.6186512775039"/>
+    <n v="13298.97128950872"/>
+    <n v="5256.3398655555793"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="381.48089155763881"/>
+    <n v="923.39312416569453"/>
+    <n v="1.5149808826027631"/>
+    <n v="3.7034525769571749"/>
+    <n v="514.67302932707867"/>
+    <n v="1"/>
+    <n v="10164.907534483191"/>
+    <n v="18128.56995523753"/>
+    <n v="8437.4881696383218"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.7333993685336964"/>
+    <n v="72.144443437621248"/>
+    <n v="2.0168156797080168"/>
+    <n v="5.0017248509263386"/>
+    <n v="420.74271164335721"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.7439190914047913"/>
+    <n v="74.71666953890508"/>
+    <n v="1.9296799285248549"/>
+    <n v="5.6237607119506006"/>
+    <n v="423.00229761534399"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.0613368189980283"/>
+    <n v="62.720056859920078"/>
+    <n v="2.2233938034918239"/>
+    <n v="8.7191362423468846"/>
+    <n v="420.7598269949662"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5.9284656844221786"/>
+    <n v="68.831170614163497"/>
+    <n v="2.0187499597366818"/>
+    <n v="6.3144991726156867"/>
+    <n v="423.75557247668849"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="14"/>
+    <n v="3.1800000000000002E-2"/>
+    <n v="25.8"/>
+    <n v="45"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6.0561830798263827"/>
+    <n v="64.102054818566103"/>
+    <n v="1.952920058142958"/>
+    <n v="9.1442469917581644"/>
+    <n v="418.91460159839693"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="0"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3.1399999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="42.3"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="64.43198788367647"/>
+    <n v="300.22111822147241"/>
+    <n v="3.3966932852172369"/>
+    <n v="8.7497414156374127"/>
+    <n v="542.90691252052"/>
+    <n v="1"/>
+    <n v="666.77342831943827"/>
+    <n v="6032.7803420599485"/>
+    <n v="1066.2117717844851"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3.1399999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="42.3"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="69.17952741979974"/>
+    <n v="282.9002270117681"/>
+    <n v="2.601733895721686"/>
+    <n v="13.190113498957761"/>
+    <n v="542.00748648921649"/>
+    <n v="1"/>
+    <n v="768.63312635177886"/>
+    <n v="5957.5595185908078"/>
+    <n v="1086.7514388359459"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3.1399999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="42.3"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="75.276789681098933"/>
+    <n v="297.22554924847009"/>
+    <n v="3.6736290429101408"/>
+    <n v="9.7297133813518872"/>
+    <n v="543.52655400105436"/>
+    <n v="1"/>
+    <n v="835.83165187925385"/>
+    <n v="6108.7041638792634"/>
+    <n v="1352.915867518383"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3.1399999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="42.3"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="77.712166142556669"/>
+    <n v="304.21170015689319"/>
+    <n v="4.1892271529192939"/>
+    <n v="8.7076449408146726"/>
+    <n v="543.15566795709037"/>
+    <n v="1"/>
+    <n v="922.19847244547123"/>
+    <n v="6335.7726309870386"/>
+    <n v="1301.35295376817"/>
+  </r>
+  <r>
+    <x v="15"/>
+    <n v="3.1399999999999997E-2"/>
+    <n v="26.2"/>
+    <n v="42.3"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="81.434421556452378"/>
+    <n v="310.71660477758542"/>
+    <n v="3.733481601915833"/>
+    <n v="6.2751736613409976"/>
+    <n v="541.50532967055346"/>
+    <n v="1"/>
+    <n v="992.23107075241899"/>
+    <n v="6147.0175739640126"/>
+    <n v="1158.9947406028471"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="434.59824413972899"/>
+    <n v="308.96933321742159"/>
+    <n v="1.5917523183690869"/>
+    <n v="7.9386132183464611"/>
+    <n v="214.72393515775519"/>
+    <n v="1"/>
+    <n v="15780.183221523939"/>
+    <n v="22677.67227924498"/>
+    <n v="8892.5185896218009"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="520.78207298295672"/>
+    <n v="306.84162492206218"/>
+    <n v="3.2045567814678062"/>
+    <n v="10.23329826784909"/>
+    <n v="122.946695425591"/>
+    <n v="1"/>
+    <n v="17568.69077875447"/>
+    <n v="16725.03374910542"/>
+    <n v="7464.749197100994"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="497.64576690631287"/>
+    <n v="451.49734959251691"/>
+    <n v="0.96056113051439795"/>
+    <n v="6.2673711540704318"/>
+    <n v="271.45313917306993"/>
+    <n v="1"/>
+    <n v="20241.470164206999"/>
+    <n v="24733.239455167979"/>
+    <n v="8555.2395826769025"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="497.18918724219247"/>
+    <n v="450.73814696790402"/>
+    <n v="1.075046447925458"/>
+    <n v="4.9150648437874196"/>
+    <n v="275.37094449995362"/>
+    <n v="1"/>
+    <n v="20010.389313303662"/>
+    <n v="25043.26172759687"/>
+    <n v="8230.2557547497127"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="477.49491223970341"/>
+    <n v="475.22572727404167"/>
+    <n v="1.3975500986284961"/>
+    <n v="4.9146873684884884"/>
+    <n v="313.53746469146148"/>
+    <n v="1"/>
+    <n v="19840.276634561818"/>
+    <n v="27033.09855777815"/>
+    <n v="8505.390085201383"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="276.42828423924101"/>
+    <n v="257.1898132626643"/>
+    <n v="2.250069140847426"/>
+    <n v="7.6216095427530206"/>
+    <n v="369.46588258937061"/>
+    <n v="1"/>
+    <n v="5909.0558370331564"/>
+    <n v="14454.349078027681"/>
+    <n v="5722.8111339877687"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="136.41620192059329"/>
+    <n v="196.8479452968395"/>
+    <n v="3.0343833484794009"/>
+    <n v="20.91053687331306"/>
+    <n v="373.21776957289711"/>
+    <n v="1"/>
+    <n v="2044.8362260413689"/>
+    <n v="13105.646743209531"/>
+    <n v="3872.032064185697"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="111.98621210619881"/>
+    <n v="157.79934028210889"/>
+    <n v="2.2270832514341938"/>
+    <n v="7.9952869871182681"/>
+    <n v="373.17639934089141"/>
+    <n v="1"/>
+    <n v="1521.905922864257"/>
+    <n v="12846.24035199352"/>
+    <n v="3516.5425216824901"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="167.70131651506821"/>
+    <n v="182.7950191436216"/>
+    <n v="2.2285973253360929"/>
+    <n v="8.6098764623501722"/>
+    <n v="454.29074828536409"/>
+    <n v="1"/>
+    <n v="2640.1140189587809"/>
+    <n v="13444.491947995741"/>
+    <n v="4565.2348881271791"/>
+  </r>
+  <r>
+    <x v="16"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="25.3"/>
+    <n v="30.7"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="144.13429633134081"/>
+    <n v="219.29749399429971"/>
+    <n v="2.7562095811658232"/>
+    <n v="7.2141750697210529"/>
+    <n v="447.05044694519518"/>
+    <n v="1"/>
+    <n v="2575.4051001900471"/>
+    <n v="13756.271716300071"/>
+    <n v="3573.701747570808"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3.6999999999999998E-2"/>
+    <n v="25.3"/>
+    <n v="34"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="148.49555112360409"/>
+    <n v="160.47892094167671"/>
+    <n v="2.0552285280964711"/>
+    <n v="13.388912905451971"/>
+    <n v="837.3795363240489"/>
+    <n v="1"/>
+    <n v="2215.6842809141449"/>
+    <n v="7886.2354923065304"/>
+    <n v="822.92727191462723"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3.6999999999999998E-2"/>
+    <n v="25.3"/>
+    <n v="34"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="67.974769221433007"/>
+    <n v="123.9910846266671"/>
+    <n v="2.6212769720601679"/>
+    <n v="10.378797348260131"/>
+    <n v="804.43300161601644"/>
+    <n v="1"/>
+    <n v="500.3750149503129"/>
+    <n v="6071.7967504948747"/>
+    <n v="626.26461364305203"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3.6999999999999998E-2"/>
+    <n v="25.3"/>
+    <n v="34"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="76.783247352936769"/>
+    <n v="133.299844792567"/>
+    <n v="2.3085190122764878"/>
+    <n v="8.496387337726123"/>
+    <n v="794.6244424641385"/>
+    <n v="1"/>
+    <n v="508.62992262189721"/>
+    <n v="6431.0289074362736"/>
+    <n v="208.7011734352389"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3.6999999999999998E-2"/>
+    <n v="25.3"/>
+    <n v="34"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="78.526658230193561"/>
+    <n v="149.427958417024"/>
+    <n v="2.3148970003880982"/>
+    <n v="13.11342132504716"/>
+    <n v="808.17947224296483"/>
+    <n v="1"/>
+    <n v="0"/>
+    <n v="5796.9243955749362"/>
+    <n v="238.00113492282571"/>
+  </r>
+  <r>
+    <x v="17"/>
+    <n v="3.6999999999999998E-2"/>
+    <n v="25.3"/>
+    <n v="34"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="80.838949915816912"/>
+    <n v="117.96033975141199"/>
+    <n v="2.8701515567834841"/>
+    <n v="15.34326924000589"/>
+    <n v="798.66419742142546"/>
+    <n v="1"/>
+    <n v="677.04633544597698"/>
+    <n v="7704.1589196102013"/>
+    <n v="245.17767671883391"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="286.94503989867599"/>
+    <n v="200.45523682291599"/>
+    <n v="3.6559958968371"/>
+    <n v="16.5996960822863"/>
+    <n v="292.4654457985306"/>
+    <n v="1"/>
+    <n v="9103.5496990102438"/>
+    <n v="20460.76698195592"/>
+    <n v="10330.7491593821"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="309.24039730514693"/>
+    <n v="192.4338469110989"/>
+    <n v="4.0947054208853002"/>
+    <n v="12.214227857851711"/>
+    <n v="289.72233060319832"/>
+    <n v="1"/>
+    <n v="10413.868135581621"/>
+    <n v="19330.345634868299"/>
+    <n v="9612.0008531400035"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="395.82976971800377"/>
+    <n v="172.30901077368841"/>
+    <n v="3.4454011901848491"/>
+    <n v="5.381420405748516"/>
+    <n v="249.0218565467184"/>
+    <n v="1"/>
+    <n v="13109.44700058578"/>
+    <n v="18063.894107021071"/>
+    <n v="8338.737787153299"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="394.27394436914773"/>
+    <n v="159.13379276642439"/>
+    <n v="4.3191953164000187"/>
+    <n v="12.225955025044721"/>
+    <n v="249.37637008120021"/>
+    <n v="1"/>
+    <n v="12084.20205169906"/>
+    <n v="16462.81536448871"/>
+    <n v="8073.0502083161919"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Air"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="389.70836163868438"/>
+    <n v="236.38011337154921"/>
+    <n v="4.1928968721386664"/>
+    <n v="7.5045593133003274"/>
+    <n v="299.89503815227607"/>
+    <n v="1"/>
+    <n v="12531.953143603911"/>
+    <n v="18463.197169922671"/>
+    <n v="8522.637443245294"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="90.566467911210808"/>
+    <n v="158.75664056211741"/>
+    <n v="4.0967640826406111"/>
+    <n v="9.1799824988463303"/>
+    <n v="352.21631159626298"/>
+    <n v="1"/>
+    <n v="1379.998913204977"/>
+    <n v="13358.72614927392"/>
+    <n v="1275.166021437723"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="72.165472646341073"/>
+    <n v="183.48941543026879"/>
+    <n v="3.730560194454986"/>
+    <n v="6.3716040593541914"/>
+    <n v="367.87651057621139"/>
+    <n v="1"/>
+    <n v="1003.299986479842"/>
+    <n v="10804.03014472392"/>
+    <n v="1914.135239792176"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="72.596346372077633"/>
+    <n v="156.36523348644189"/>
+    <n v="2.8652704085236991"/>
+    <n v="7.4741107242644249"/>
+    <n v="377.07835931192221"/>
+    <n v="1"/>
+    <n v="1120.724489624524"/>
+    <n v="10750.602270110319"/>
+    <n v="1537.909274573075"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="83.874087112857296"/>
+    <n v="151.058755479979"/>
+    <n v="2.643322846671861"/>
+    <n v="10.67084555779047"/>
+    <n v="338.30752989977799"/>
+    <n v="1"/>
+    <n v="1419.1151009834291"/>
+    <n v="9648.6523562049479"/>
+    <n v="757.28486352166669"/>
+  </r>
+  <r>
+    <x v="18"/>
+    <n v="4.1099999999999998E-2"/>
+    <n v="24.6"/>
+    <n v="30.8"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="64.537614638584955"/>
+    <n v="143.620798505799"/>
+    <n v="2.4529302326980278"/>
+    <n v="10.019571360804949"/>
+    <n v="363.25542509870928"/>
+    <n v="1"/>
+    <n v="761.68694926458602"/>
+    <n v="9253.9187825795161"/>
+    <n v="425.15088665188171"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="24.7"/>
+    <n v="34.5"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="188.63363831987149"/>
+    <n v="231.3959276825704"/>
+    <n v="2.3955574301484819"/>
+    <n v="15.298802811954619"/>
+    <n v="318.01855006779732"/>
+    <n v="1"/>
+    <n v="4044.4009322129832"/>
+    <n v="4977.2283192663781"/>
+    <n v="2024.960088193789"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="24.7"/>
+    <n v="34.5"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="142.90397891603081"/>
+    <n v="217.18159202329289"/>
+    <n v="1.9676161806305541"/>
+    <n v="9.546349736811484"/>
+    <n v="264.34318289467768"/>
+    <n v="1"/>
+    <n v="2646.5516935566989"/>
+    <n v="4732.5848934041314"/>
+    <n v="725.45327389045781"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="24.7"/>
+    <n v="34.5"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="86.105444422202496"/>
+    <n v="140.6952906236165"/>
+    <n v="2.115455762832668"/>
+    <n v="4.3502803536448393"/>
+    <n v="257.99016832826402"/>
+    <n v="1"/>
+    <n v="763.78930594226335"/>
+    <n v="4068.9544508352819"/>
+    <n v="584.06303150255076"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="24.7"/>
+    <n v="34.5"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="31.954308556531259"/>
+    <n v="151.26774141320129"/>
+    <n v="2.258101642949931"/>
+    <n v="9.8291356956436324"/>
+    <n v="307.93722640603761"/>
+    <n v="1"/>
+    <n v="-26.437481943460739"/>
+    <n v="4270.0119789864366"/>
+    <n v="186.5038037192941"/>
+  </r>
+  <r>
+    <x v="19"/>
+    <n v="3.7400000000000003E-2"/>
+    <n v="24.7"/>
+    <n v="34.5"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="32.820986555014201"/>
+    <n v="179.94924778685069"/>
+    <n v="3.142932335676484"/>
+    <n v="12.246830056128671"/>
+    <n v="273.89857287073579"/>
+    <n v="1"/>
+    <n v="63.787799625753962"/>
+    <n v="3554.7111576794409"/>
+    <n v="265.51570922110369"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="4.0500000000000001E-2"/>
+    <n v="25.5"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="261.4663348190428"/>
+    <n v="301.90658448858773"/>
+    <n v="3.3370560149058011"/>
+    <n v="14.573895688758"/>
+    <n v="528.91759569791714"/>
+    <n v="1"/>
+    <n v="9264.8420173057966"/>
+    <n v="11008.95416380106"/>
+    <n v="5222.1180718137384"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="4.0500000000000001E-2"/>
+    <n v="25.5"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="191.88055333992341"/>
+    <n v="205.05409605755321"/>
+    <n v="2.2237929866753081"/>
+    <n v="5.4245109553005122"/>
+    <n v="473.20531034458429"/>
+    <n v="1"/>
+    <n v="4982.385750494409"/>
+    <n v="8827.5502831960312"/>
+    <n v="3571.201592273716"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="4.0500000000000001E-2"/>
+    <n v="25.5"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="225.39882572365411"/>
+    <n v="216.87638246654029"/>
+    <n v="3.272373805652419"/>
+    <n v="11.03044257915284"/>
+    <n v="390.75582180515221"/>
+    <n v="1"/>
+    <n v="6339.5326007151953"/>
+    <n v="8693.2775983118681"/>
+    <n v="3988.9488724705379"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="4.0500000000000001E-2"/>
+    <n v="25.5"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="173.5836760518682"/>
+    <n v="211.53670504201449"/>
+    <n v="2.6219300962080538"/>
+    <n v="17.30411089083039"/>
+    <n v="575.27267731449797"/>
+    <n v="1"/>
+    <n v="4074.28456729972"/>
+    <n v="9212.7933790940515"/>
+    <n v="2843.6179338337738"/>
+  </r>
+  <r>
+    <x v="20"/>
+    <n v="4.0500000000000001E-2"/>
+    <n v="25.5"/>
+    <n v="41.4"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="80.831538587376031"/>
+    <n v="159.54655771620591"/>
+    <n v="2.422525353135355"/>
+    <n v="8.5599223209979769"/>
+    <n v="516.45731174544596"/>
+    <n v="1"/>
+    <n v="1190.578207624794"/>
+    <n v="4165.2652248097866"/>
+    <n v="321.038232753861"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="3.6799999999999999E-2"/>
+    <n v="25.1"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="7.4022375449076208"/>
+    <n v="152.88832498100561"/>
+    <n v="2.8381400264465739"/>
+    <n v="12.67079768522475"/>
+    <n v="162.86426436864639"/>
+    <n v="1"/>
+    <n v="-39.216460470415143"/>
+    <n v="3155.0565956027549"/>
+    <n v="70.684900273836149"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="3.6799999999999999E-2"/>
+    <n v="25.1"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="13.76285684752134"/>
+    <n v="122.50317260246899"/>
+    <n v="2.503061874040506"/>
+    <n v="8.9836116280177034"/>
+    <n v="126.4739600446014"/>
+    <n v="1"/>
+    <n v="3.332001136918993"/>
+    <n v="2608.4753783386859"/>
+    <n v="-211.74488140221729"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="3.6799999999999999E-2"/>
+    <n v="25.1"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="13.8713534332237"/>
+    <n v="178.19405020618751"/>
+    <n v="2.18088403845598"/>
+    <n v="8.3291838064815238"/>
+    <n v="121.0451906272433"/>
+    <n v="1"/>
+    <n v="6.1335731719132864"/>
+    <n v="2585.979431132962"/>
+    <n v="-35.533858370697203"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="3.6799999999999999E-2"/>
+    <n v="25.1"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="8.2455829455739149E-2"/>
+    <n v="144.00370330139319"/>
+    <n v="3.5237242345709441"/>
+    <n v="10.94966570320749"/>
+    <n v="171.77665217734781"/>
+    <n v="1"/>
+    <n v="-1.2281455935389829"/>
+    <n v="3112.173696241844"/>
+    <n v="64.930928081401333"/>
+  </r>
+  <r>
+    <x v="21"/>
+    <n v="3.6799999999999999E-2"/>
+    <n v="25.1"/>
+    <n v="31.9"/>
+    <s v="Water"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="5.6908604488522769"/>
+    <n v="110.51502168721839"/>
+    <n v="3.2129905681553339"/>
+    <n v="17.486743511922281"/>
+    <n v="162.11334291767881"/>
+    <n v="1"/>
+    <n v="-4.9613371990318944"/>
+    <n v="2941.345097148379"/>
+    <n v="-144.52674609137151"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="290.44085068182972"/>
+    <n v="394.74718793507918"/>
+    <n v="1.6809107960824761"/>
+    <n v="5.752382771694645"/>
+    <n v="251.53975710083731"/>
+    <n v="1"/>
+    <n v="12229.753981375379"/>
+    <n v="14024.114087718221"/>
+    <n v="6589.4429159361453"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="394.32402304068961"/>
+    <n v="382.99560236385878"/>
+    <n v="3.0926768271002039"/>
+    <n v="3.959871657867347"/>
+    <n v="198.73101316775191"/>
+    <n v="1"/>
+    <n v="17590.307201755681"/>
+    <n v="12787.891488928681"/>
+    <n v="6641.1327207242648"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="380.55204642715029"/>
+    <n v="376.91035513177218"/>
+    <n v="1.9911941751667011"/>
+    <n v="7.1016832962774838"/>
+    <n v="150.3793521071411"/>
+    <n v="1"/>
+    <n v="14370.325290877179"/>
+    <n v="10219.1355173751"/>
+    <n v="5285.5709793570986"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="381.97982488698278"/>
+    <n v="294.96755597734591"/>
+    <n v="3.4452027326266972"/>
+    <n v="14.964759803096991"/>
+    <n v="143.88004458532541"/>
+    <n v="1"/>
+    <n v="13611.95879174756"/>
+    <n v="9551.6385838802635"/>
+    <n v="5151.7438791273034"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="403.97854364082309"/>
+    <n v="421.18771985123288"/>
+    <n v="2.8913885447368459"/>
+    <n v="7.9551847268311704"/>
+    <n v="201.16320270872191"/>
+    <n v="1"/>
+    <n v="17689.503379723181"/>
+    <n v="11899.30157430259"/>
+    <n v="5099.0792247940708"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="210.49641998432969"/>
+    <n v="312.45895081042642"/>
+    <n v="2.9437063991153352"/>
+    <n v="19.574460432435291"/>
+    <n v="529.62349669272419"/>
+    <n v="1"/>
+    <n v="7451.2591746456483"/>
+    <n v="6119.2491391319472"/>
+    <n v="2047.580455909791"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="258.5552572053038"/>
+    <n v="352.59393734146528"/>
+    <n v="3.375742035235572"/>
+    <n v="8.3170637276602299"/>
+    <n v="411.40755969227922"/>
+    <n v="1"/>
+    <n v="9422.4565495203424"/>
+    <n v="5244.7191915094363"/>
+    <n v="1046.890477720902"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="264.27596549332708"/>
+    <n v="287.16986297837548"/>
+    <n v="2.516885765996443"/>
+    <n v="9.0093892662659378"/>
+    <n v="400.63493538545742"/>
+    <n v="1"/>
+    <n v="9346.2845063108125"/>
+    <n v="4459.8215335347304"/>
+    <n v="899.45788326015179"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="268.26065413785062"/>
+    <n v="301.15778355893639"/>
+    <n v="2.4464647484036681"/>
+    <n v="24.93028829934978"/>
+    <n v="526.97157940343448"/>
+    <n v="1"/>
+    <n v="9992.6597072081167"/>
+    <n v="6363.1895666440141"/>
+    <n v="1275.8898812622481"/>
+  </r>
+  <r>
+    <x v="22"/>
+    <n v="3.4599999999999999E-2"/>
+    <n v="25"/>
+    <n v="41.7"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="290.66678073516402"/>
+    <n v="331.82066142474878"/>
+    <n v="2.9207517711009969"/>
+    <n v="13.81454690946911"/>
+    <n v="503.57840817945117"/>
+    <n v="1"/>
+    <n v="11055.284900531989"/>
+    <n v="6186.0339823989407"/>
+    <n v="1271.1470327284501"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="538.66267115148219"/>
+    <n v="335.50806576551309"/>
+    <n v="0.97838180103292183"/>
+    <n v="9.1236013744827744"/>
+    <n v="394.9296446518178"/>
+    <n v="1"/>
+    <n v="21353.56994907133"/>
+    <n v="21848.485725209001"/>
+    <n v="11575.631434874569"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="536.66550351364924"/>
+    <n v="323.97224297601042"/>
+    <n v="0.67621018315961934"/>
+    <n v="4.9838329499414096"/>
+    <n v="363.52687384965708"/>
+    <n v="1"/>
+    <n v="21417.63012452544"/>
+    <n v="21080.108528463501"/>
+    <n v="10975.096655619051"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="549.03621873164309"/>
+    <n v="315.04901015437281"/>
+    <n v="0.62044498748177057"/>
+    <n v="1.857562624713462"/>
+    <n v="292.85156622770131"/>
+    <n v="1"/>
+    <n v="20854.050898457321"/>
+    <n v="19119.446129814649"/>
+    <n v="11382.731530890271"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="545.5544442017557"/>
+    <n v="317.48253994553852"/>
+    <n v="1.335875481239118"/>
+    <n v="1.4429270826441769"/>
+    <n v="278.59951392184217"/>
+    <n v="1"/>
+    <n v="20749.157242043129"/>
+    <n v="18671.28468157562"/>
+    <n v="8385.669532745791"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Air"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="610.46817690401826"/>
+    <n v="392.00718426622598"/>
+    <n v="0.59336239976559968"/>
+    <n v="4.9195656781228188"/>
+    <n v="360.29580884075239"/>
+    <n v="1"/>
+    <n v="28008.79501861547"/>
+    <n v="20783.091725512932"/>
+    <n v="5932.7631886723721"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="451.50465064349447"/>
+    <n v="336.14963125836948"/>
+    <n v="4.8854595639722893"/>
+    <n v="3.6172087940327602"/>
+    <n v="305.12863028893332"/>
+    <n v="1"/>
+    <n v="16190.76193225617"/>
+    <n v="9501.0227026673874"/>
+    <n v="2783.6803417373249"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="463.21083815484099"/>
+    <n v="270.77721424034331"/>
+    <n v="4.9293032750682384"/>
+    <n v="3.9012040340282672"/>
+    <n v="296.77433651810929"/>
+    <n v="1"/>
+    <n v="16980.130010985358"/>
+    <n v="8957.2534788040321"/>
+    <n v="2151.710079041175"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="501.42606043758252"/>
+    <n v="361.79524087647872"/>
+    <n v="4.6183630662464772"/>
+    <n v="6.1701178137331194"/>
+    <n v="379.9980104764486"/>
+    <n v="1"/>
+    <n v="20118.794819976691"/>
+    <n v="9822.2929486991288"/>
+    <n v="3899.9677277401779"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="509.14994046532809"/>
+    <n v="399.96961069665292"/>
+    <n v="2.8702077833113191"/>
+    <n v="4.1440954869867479"/>
+    <n v="432.96991473698063"/>
+    <n v="1"/>
+    <n v="20268.81003079065"/>
+    <n v="10453.936966334841"/>
+    <n v="4602.9292371651454"/>
+  </r>
+  <r>
+    <x v="23"/>
+    <n v="3.0499999999999999E-2"/>
+    <n v="25"/>
+    <n v="33.9"/>
+    <s v="Water"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="505.46457183317062"/>
+    <n v="345.83732493346002"/>
+    <n v="2.5945704178124922"/>
+    <n v="3.555113927794006"/>
+    <n v="367.27355780847643"/>
+    <n v="1"/>
+    <n v="24134.733515079341"/>
+    <n v="12533.757585339021"/>
+    <n v="3530.0208655538659"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:C9" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="24">
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="14"/>
+        <item x="2"/>
+        <item x="23"/>
+        <item x="3"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="17"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="6"/>
+        <item x="20"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="21"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="22"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="6" item="1" hier="-1"/>
+    <pageField fld="5" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Average of Pulloff Force (µN)" fld="7" subtotal="average" baseField="0" baseItem="0"/>
+    <dataField name="StdDev of Pulloff Force (µN)2" fld="7" subtotal="stdDev" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -586,9 +3875,275 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="3" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="24" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>564.91932394717173</v>
+      </c>
+      <c r="G4">
+        <v>47.98024550048742</v>
+      </c>
+      <c r="H4">
+        <f>G4/F4</f>
+        <v>8.4932916022844848E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>564.91932394717173</v>
+      </c>
+      <c r="C5" s="4">
+        <v>47.98024550048742</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>490.31081247680169</v>
+      </c>
+      <c r="G5">
+        <v>32.086267234204804</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H13" si="0">G5/F5</f>
+        <v>6.5440668281658412E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4">
+        <v>556.0774029005097</v>
+      </c>
+      <c r="C6" s="4">
+        <v>30.817048652785541</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>460.6041461846761</v>
+      </c>
+      <c r="G6">
+        <v>27.144439538152465</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>5.8932251832724679E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>306.87237244532747</v>
+      </c>
+      <c r="C7" s="4">
+        <v>57.372462836435083</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>383.12921936092636</v>
+      </c>
+      <c r="G7">
+        <v>48.425400112859712</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.12639443212823878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4">
+        <v>360.59438792691634</v>
+      </c>
+      <c r="C8" s="4">
+        <v>16.910694502933815</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8">
+        <v>556.0774029005097</v>
+      </c>
+      <c r="G8">
+        <v>30.817048652785541</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>5.5418631456777896E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4">
+        <v>370.25505773549509</v>
+      </c>
+      <c r="C9" s="4">
+        <v>45.635497096415229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>485.54203670217896</v>
+      </c>
+      <c r="G9">
+        <v>32.342088562688474</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>6.6610274946237905E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>355.19950258593178</v>
+      </c>
+      <c r="G10">
+        <v>52.771685106580883</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.14856914134842875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>306.87237244532747</v>
+      </c>
+      <c r="G11">
+        <v>57.372462836435083</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.18695870983516638</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>360.59438792691634</v>
+      </c>
+      <c r="G12">
+        <v>16.910694502933815</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>4.689672127221569E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>370.25505773549509</v>
+      </c>
+      <c r="G13">
+        <v>45.635497096415229</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.1232542166352163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f>AVERAGE(B5:B9)</f>
+        <v>431.74370899108408</v>
+      </c>
+      <c r="G16">
+        <f>_xlfn.STDEV.P(B5:B9)</f>
+        <v>107.35971560314583</v>
+      </c>
+      <c r="H16">
+        <f>G16/F16</f>
+        <v>0.24866538496653096</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>